<commit_message>
Einstine created Hlookup file
</commit_message>
<xml_diff>
--- a/Vlookup.xlsx
+++ b/Vlookup.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics- ARC\Excel Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D85FD88A-9EED-467B-B02C-2A49EC2DC72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C649D685-FE5E-4911-8F42-B86F2852367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{B2A94395-A615-45CD-AB88-0BA8982DE4FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{B2A94395-A615-45CD-AB88-0BA8982DE4FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Task 1" sheetId="1" r:id="rId1"/>
     <sheet name="Vlookup" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1047,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7512FFB9-015C-4585-BBDD-5DE235D235CC}">
   <dimension ref="B3:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
@@ -1162,7 +1163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="29">
+    <row r="30" spans="2:7">
       <c r="B30" s="9" t="s">
         <v>15</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="76" spans="2:9" ht="29">
+    <row r="76" spans="2:9">
       <c r="B76" s="20" t="s">
         <v>52</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="29">
+    <row r="77" spans="2:9">
       <c r="B77" s="20" t="s">
         <v>55</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="29">
+    <row r="80" spans="2:9">
       <c r="B80" s="20" t="s">
         <v>62</v>
       </c>
@@ -1612,4 +1613,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E103C3A2-E3C2-4440-ABC7-57B4024C2613}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>